<commit_message>
new leetcode files inserted
</commit_message>
<xml_diff>
--- a/Interview Prep/2020/Leetcode Logging.xlsx
+++ b/Interview Prep/2020/Leetcode Logging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\burwi\Notebook\Interview Prep\2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2C5144-218D-40B3-B967-5B9FEB2F7545}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7C87F25-521D-4CD2-BFE1-906B5C8D2097}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{30200DC3-57F2-459D-AA27-92FFE8D9BF4E}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,10 +49,10 @@
     <t>Dynamic Programming -- Taking Larger Problem and breaking to each palindrome case</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Beyond me at the moment</t>
+    <t>2 hrs?</t>
+  </si>
+  <si>
+    <t>Data Structures -- use set to parse through to find attributes</t>
   </si>
 </sst>
 </file>
@@ -406,7 +407,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>